<commit_message>
Foglio di lavoro aggiornato
</commit_message>
<xml_diff>
--- a/Foglio di Lavoro.xlsx
+++ b/Foglio di Lavoro.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sponky\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sponky\Desktop\Nuova cartella (2)\AI-Car\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BDEB92-51DF-4AB1-875C-43FF44AAE86E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C0C46A-BDBE-42F8-A638-31C73594A916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="116">
   <si>
     <t>Matricola</t>
   </si>
@@ -330,28 +330,58 @@
     <t>Addestramento con scarsi risultati</t>
   </si>
   <si>
-    <t>Ho fatto partire un addestramento ma non ho ottenuto nessun risultato (0 ore conteggiate)</t>
-  </si>
-  <si>
     <t>Creazione metodo CheckPedoneSuperato</t>
   </si>
   <si>
     <t>Creazione di questo metodo per verificare se la macchina ha superato il pedone. Ho effettuato test ma ci sono ancora imperfezioni da risolvere</t>
   </si>
   <si>
-    <t>//Cosa ho fatto qui?</t>
-  </si>
-  <si>
     <t>Presa visione di un progetto e l'ho replicato per cercare di acquisire nuove informazioni riguardo l'utilizzo di ML Agents</t>
-  </si>
-  <si>
-    <t>Mancanza di internet…</t>
   </si>
   <si>
     <t>Modifica CheckPedoneSuperato e nuova sessione di addestramento</t>
   </si>
   <si>
     <t>Nuova sessione di addestramento che ha portato ottimi risultati. Manca una sola cosa da correggere: la macchina deve fermarsi completamente quando incontra un pedone e non deve proseguire lentamente come fa ora.</t>
+  </si>
+  <si>
+    <t>Creazione Menu</t>
+  </si>
+  <si>
+    <t>Creazione Scena Menu e Bug Fix</t>
+  </si>
+  <si>
+    <t>Addestramento finale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixato il bug per cui la macchina tendeva ad avanzare lentamente nonostante vedesse il pedone. Ora la macchina si ferma perfettamente in prossimità di un pedone e, quindi, dell'attraversamento pedonale. </t>
+  </si>
+  <si>
+    <t>Addestramento finale + Bug Fix</t>
+  </si>
+  <si>
+    <t>Addestramento finale con qualche leggera modifica al codice per migliorarne la leggibilità e la comprensione.</t>
+  </si>
+  <si>
+    <t>Modifica al prefab CarAgent</t>
+  </si>
+  <si>
+    <t>Modifica al componente RayPerceptionSensor</t>
+  </si>
+  <si>
+    <t>Dopo vari test ho modificato il componente RayPerceptionSensor dell'oggetto CarAgente in modo da avere una visuale più ampia. Sistemata anche l'altezza dei raggi e la grandezza delle sfere. Altro addestramento con risultati leggermente migliori.</t>
+  </si>
+  <si>
+    <t>Sessione di training</t>
+  </si>
+  <si>
+    <t>Giornata di training per prendere appunti su ciò che non va</t>
+  </si>
+  <si>
+    <t>Giornata dedicata completamente al training per capire su quali punti intervenire per migliorare i risultati.</t>
+  </si>
+  <si>
+    <t>Addestramento ma nessun risultato positivo (0 ore conteggiate)</t>
   </si>
 </sst>
 </file>
@@ -2904,7 +2934,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
@@ -3009,10 +3039,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
@@ -3066,13 +3096,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -4403,7 +4433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5478,8 +5508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5562,7 +5592,7 @@
         <v>31</v>
       </c>
       <c r="E6" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5592,7 +5622,7 @@
         <v>46</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>29</v>
@@ -6082,11 +6112,17 @@
         <v>44000</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="8"/>
+      <c r="C41" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
@@ -6094,11 +6130,17 @@
         <v>44001</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="8"/>
+      <c r="C42" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="8">
+        <v>6</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
@@ -6250,7 +6292,7 @@
         <v>97</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="E52" s="8">
         <v>0</v>
@@ -6333,10 +6375,10 @@
         <v>95</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E57" s="10">
         <v>4</v>
@@ -6348,7 +6390,7 @@
         <v>44017</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
@@ -6363,10 +6405,10 @@
         <v>70</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E59" s="10">
         <v>6</v>
@@ -6377,30 +6419,52 @@
         <f>riassuntoOreProgetto!A58</f>
         <v>44019</v>
       </c>
-      <c r="B60" s="27"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="8"/>
+      <c r="B60" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E60" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>riassuntoOreProgetto!A59</f>
         <v>44020</v>
       </c>
-      <c r="B61" s="27"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="8"/>
+      <c r="B61" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E61" s="8">
+        <v>6</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>riassuntoOreProgetto!A60</f>
         <v>44021</v>
       </c>
-      <c r="B62" s="28"/>
-      <c r="C62" s="11"/>
+      <c r="B62" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="D62" s="11"/>
-      <c r="E62" s="10"/>
+      <c r="E62" s="10">
+        <v>7</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
@@ -9590,8 +9654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A77" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9680,7 +9744,7 @@
       </c>
       <c r="B4" s="21">
         <f>TabellaEstesa!E6</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -10555,7 +10619,7 @@
       </c>
       <c r="B39" s="21">
         <f>TabellaEstesa!E41</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -10580,7 +10644,7 @@
       </c>
       <c r="B40" s="21">
         <f>TabellaEstesa!E42</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -11030,7 +11094,7 @@
       </c>
       <c r="B58" s="21">
         <f>TabellaEstesa!E60</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -11055,7 +11119,7 @@
       </c>
       <c r="B59" s="21">
         <f>TabellaEstesa!E61</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -11080,7 +11144,7 @@
       </c>
       <c r="B60" s="21">
         <f>TabellaEstesa!E62</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -12455,7 +12519,7 @@
       </c>
       <c r="B115" s="22">
         <f>SUM(B2:B114)</f>
-        <v>170.5</v>
+        <v>202.5</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
@@ -32911,7 +32975,7 @@
       </c>
       <c r="B4" s="18">
         <f>SUM(riassuntoOreProgetto!B2:B114)</f>
-        <v>170.5</v>
+        <v>202.5</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>

</xml_diff>